<commit_message>
unit view range done, unit move range works (slow)
</commit_message>
<xml_diff>
--- a/other/calculations.xlsx
+++ b/other/calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10965" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="geometry" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>&lt;= camera angle from ground parallel</t>
   </si>
   <si>
-    <t>per move</t>
-  </si>
-  <si>
     <t>per short</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>wm mission failes</t>
+  </si>
+  <si>
+    <t>moves</t>
   </si>
 </sst>
 </file>
@@ -559,29 +559,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -602,8 +602,16 @@
         <f t="shared" ref="G2:G14" si="1">B2-F2*C2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>B2/(D2)</f>
+        <v>9.1428571428571423</v>
+      </c>
+      <c r="J2">
+        <f>B2/7</f>
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -624,8 +632,16 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H14" si="2">B3/(D3)</f>
+        <v>9.1428571428571423</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J14" si="3">B3/7</f>
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -646,8 +662,16 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>9.1428571428571423</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -668,8 +692,16 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>9.1428571428571423</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -690,8 +722,16 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>9.1428571428571423</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -712,8 +752,16 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>9.1428571428571423</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -724,7 +772,7 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -734,8 +782,16 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>8.875</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>10.142857142857142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -746,7 +802,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -756,8 +812,16 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>8.875</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>10.142857142857142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -768,7 +832,7 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -778,8 +842,16 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>8.875</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>10.142857142857142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -790,7 +862,7 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -800,8 +872,16 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>9.75</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>11.142857142857142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -812,7 +892,7 @@
         <v>15</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -822,8 +902,16 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>11.142857142857142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -834,7 +922,7 @@
         <v>15</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -844,8 +932,16 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>11.142857142857142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -856,7 +952,7 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -865,6 +961,14 @@
       <c r="G14">
         <f t="shared" si="1"/>
         <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>11.142857142857142</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -887,120 +991,120 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>640</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>640</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>176</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>160</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>436</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>340</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>340</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unit move, attack, some spec actions, ambient sounds done
</commit_message>
<xml_diff>
--- a/other/calculations.xlsx
+++ b/other/calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="geometry" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>y</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>moves</t>
+  </si>
+  <si>
+    <t>MM_LOAD.LZ</t>
+  </si>
+  <si>
+    <t>load position screen</t>
+  </si>
+  <si>
+    <t>OPT_BAR.LZ</t>
+  </si>
+  <si>
+    <t>looks like chunk of window frame?</t>
   </si>
 </sst>
 </file>
@@ -561,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,10 +990,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,6 +1119,28 @@
         <v>34</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>402</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
events shown in editor mode
</commit_message>
<xml_diff>
--- a/other/calculations.xlsx
+++ b/other/calculations.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>y</t>
   </si>
@@ -146,6 +146,27 @@
   </si>
   <si>
     <t>looks like chunk of window frame?</t>
+  </si>
+  <si>
+    <t>mission options frame</t>
+  </si>
+  <si>
+    <t>RAM2VERT.DTA</t>
+  </si>
+  <si>
+    <t>frame vert part</t>
+  </si>
+  <si>
+    <t>RAM2HORZ.DTA</t>
+  </si>
+  <si>
+    <t>frame horz part</t>
+  </si>
+  <si>
+    <t>RAM2ROH.DTA</t>
+  </si>
+  <si>
+    <t>frame corner</t>
   </si>
 </sst>
 </file>
@@ -990,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,6 +1162,50 @@
         <v>39</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>436</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add spelldata loader panel, add some loaders error protections
</commit_message>
<xml_diff>
--- a/other/calculations.xlsx
+++ b/other/calculations.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10965" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10965" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="geometry" sheetId="1" r:id="rId1"/>
     <sheet name="kpt.alex" sheetId="2" r:id="rId2"/>
     <sheet name="List1" sheetId="3" r:id="rId3"/>
+    <sheet name="exp" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>y</t>
   </si>
@@ -167,6 +168,15 @@
   </si>
   <si>
     <t>frame corner</t>
+  </si>
+  <si>
+    <t>next level</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -203,8 +213,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -220,6 +231,1115 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.2409219160104987"/>
+                  <c:y val="0.22081437736949547"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="cs-CZ"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>exp!$A$30:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>exp!$C$30:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2107</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5319</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10138</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16563</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>exp!$A$30:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>exp!$D$30:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>631.84655785531265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1465.3204756903931</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2661.5338178240459</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4228.464024802015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6172.384658132557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8498.4863115812968</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11211.206542717537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14314.427309850129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17811.60292724118</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21705.847912566867</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25999.999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="318630992"/>
+        <c:axId val="318627632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="318630992"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="318627632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="318627632"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="318630992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graf 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1013,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -1209,4 +2329,685 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>96</v>
+      </c>
+      <c r="C2">
+        <v>520</v>
+      </c>
+      <c r="H2" s="1">
+        <f>C2/A2^2.5</f>
+        <v>520</v>
+      </c>
+      <c r="J2">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1047</v>
+      </c>
+      <c r="C3">
+        <v>3188</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H13" si="0">C3/A3^2.5</f>
+        <v>563.56410460567838</v>
+      </c>
+      <c r="J3">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5736</v>
+      </c>
+      <c r="C4">
+        <v>9632</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>617.89308809271927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>14063</v>
+      </c>
+      <c r="C5">
+        <v>20373</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>636.65625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>24067</v>
+      </c>
+      <c r="C6">
+        <v>35410</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>633.43333666614046</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>42870</v>
+      </c>
+      <c r="C7">
+        <v>54743</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>620.79822680175721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>63086</v>
+      </c>
+      <c r="C8">
+        <v>78372</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>604.5271771159014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>83582</v>
+      </c>
+      <c r="C9">
+        <v>106298</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>587.2190361450597</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>118842</v>
+      </c>
+      <c r="C10">
+        <v>138520</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>570.0411522633741</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>144033</v>
+      </c>
+      <c r="C11">
+        <v>175038</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>553.51875708055229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>179064</v>
+      </c>
+      <c r="C12">
+        <v>215852</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>537.86633677520183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>221564</v>
+      </c>
+      <c r="C13">
+        <f>200*J3</f>
+        <v>276000</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>553.29400797339144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1200</v>
+      </c>
+      <c r="H16" s="1">
+        <f>C16/A16^2.5</f>
+        <v>1200</v>
+      </c>
+      <c r="J16">
+        <v>1200</v>
+      </c>
+      <c r="K16" s="1">
+        <f>$L$16*A16^2.5</f>
+        <v>150</v>
+      </c>
+      <c r="L16">
+        <v>150</v>
+      </c>
+      <c r="M16">
+        <f>K16/A16^2.5</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>7225</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" ref="H17:H27" si="1">C17/A17^2.5</f>
+        <v>1277.2116235182013</v>
+      </c>
+      <c r="J17">
+        <v>3100</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" ref="K17:K27" si="2">$L$16*A17^2.5</f>
+        <v>848.52813742385706</v>
+      </c>
+      <c r="L17">
+        <v>130</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17:M27" si="3">K17/A17^2.5</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>21700</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>1392.0556490460972</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="2"/>
+        <v>2338.2685902179851</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>45825</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>1432.03125</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="2"/>
+        <v>4800</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>79600</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
+        <v>1423.9280880718663</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="2"/>
+        <v>8385.2549156242094</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>123025</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>1395.131831508799</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="2"/>
+        <v>13227.244611029157</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>176100</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>1358.3580346311212</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="2"/>
+        <v>19446.272136324733</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>238825</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>1319.3341954443536</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="2"/>
+        <v>27152.900397563419</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>311200</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>1280.6584362139909</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="2"/>
+        <v>36450.000000000029</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>150.00000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>394225</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>1246.648910579878</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="2"/>
+        <v>47434.164902525736</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>484900</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>1208.2880246756822</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="2"/>
+        <v>60196.739944950525</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <f>J17*200</f>
+        <v>620000</v>
+      </c>
+      <c r="H27" s="1">
+        <f>C27/A27^2.5</f>
+        <v>1242.9068295054444</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="2"/>
+        <v>74824.594886975494</v>
+      </c>
+      <c r="L27">
+        <f>L17*200</f>
+        <v>26000</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>150</v>
+      </c>
+      <c r="D30">
+        <f>$O$30*A30^$O$31</f>
+        <v>150</v>
+      </c>
+      <c r="H30" s="1">
+        <f>C30/A30^2.5</f>
+        <v>150</v>
+      </c>
+      <c r="J30">
+        <v>150</v>
+      </c>
+      <c r="N30" t="s">
+        <v>49</v>
+      </c>
+      <c r="O30">
+        <f>J30</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:D41" si="4">$O$30*A31^$O$31</f>
+        <v>631.84655785531265</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" ref="H31:H41" si="5">C31/A31^2.5</f>
+        <v>88.38834764831843</v>
+      </c>
+      <c r="J31">
+        <v>130</v>
+      </c>
+      <c r="N31" t="s">
+        <v>48</v>
+      </c>
+      <c r="O31">
+        <f>LN(J31*200/J30)/LN(12)</f>
+        <v>2.0746117458163589</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>1103</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="4"/>
+        <v>1465.3204756903931</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="5"/>
+        <v>70.75748299068411</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>2107</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="4"/>
+        <v>2661.5338178240459</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="5"/>
+        <v>65.84375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>3512</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="4"/>
+        <v>4228.464024802015</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="5"/>
+        <v>62.824565895834098</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>5319</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="4"/>
+        <v>6172.384658132557</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="5"/>
+        <v>60.318684916035785</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>7528</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="4"/>
+        <v>8498.4863115812968</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="5"/>
+        <v>58.067684751295182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>10138</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="4"/>
+        <v>11211.206542717537</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="5"/>
+        <v>56.005066778665785</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>13150</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="4"/>
+        <v>14314.427309850129</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="5"/>
+        <v>54.115226337448519</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>16563</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="4"/>
+        <v>17811.60292724118</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="5"/>
+        <v>52.376804885368813</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>20378</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="4"/>
+        <v>21705.847912566867</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="5"/>
+        <v>50.778497353765829</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <f>J31*200</f>
+        <v>26000</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="4"/>
+        <v>25999.999999999989</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="5"/>
+        <v>52.121899301841218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>